<commit_message>
Barclays DAD intervju utskriven
</commit_message>
<xml_diff>
--- a/Material/AgileScalingKnowledgebase(ASK-5.1).xlsx
+++ b/Material/AgileScalingKnowledgebase(ASK-5.1).xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\SkyDrive\Documents\ASK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Documents\GitHub\Kandi2\Kandi2\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Sheet1(Custom Criteria)'!$1:$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Sheet2(Approach Comparison)'!$1:$14</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1269,7 +1269,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2105,27 +2105,39 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="49" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="49" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2191,18 +2203,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="49" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="63">
@@ -2270,40 +2270,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="60">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF8000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="57">
     <dxf>
       <font>
         <color rgb="FFFF6FCF"/>
@@ -3308,18 +3275,18 @@
       <c r="Q1" s="5"/>
     </row>
     <row r="3" spans="1:21" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
       <c r="K3" s="36"/>
       <c r="L3" s="36"/>
       <c r="M3" s="36"/>
@@ -3333,17 +3300,17 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="64"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="66"/>
       <c r="K4" s="35"/>
       <c r="L4" s="35"/>
       <c r="M4" s="35"/>
@@ -3357,17 +3324,17 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="64"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="66"/>
       <c r="K5" s="35"/>
       <c r="L5" s="35"/>
       <c r="M5" s="35"/>
@@ -3381,17 +3348,17 @@
       <c r="A6" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="64" t="s">
         <v>118</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="63"/>
-      <c r="J6" s="64"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="66"/>
       <c r="K6" s="35"/>
       <c r="L6" s="35"/>
       <c r="M6" s="35"/>
@@ -3405,17 +3372,17 @@
       <c r="A7" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="64"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="66"/>
       <c r="K7" s="35"/>
       <c r="L7" s="35"/>
       <c r="M7" s="35"/>
@@ -3429,17 +3396,17 @@
       <c r="A8" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="63"/>
-      <c r="J8" s="64"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="66"/>
       <c r="K8" s="35"/>
       <c r="L8" s="35"/>
       <c r="M8" s="35"/>
@@ -3453,17 +3420,17 @@
       <c r="A9" s="54" t="s">
         <v>173</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="64" t="s">
         <v>174</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="64"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="66"/>
       <c r="K9" s="35"/>
       <c r="L9" s="35"/>
       <c r="M9" s="35"/>
@@ -3477,17 +3444,17 @@
       <c r="A10" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="64" t="s">
         <v>172</v>
       </c>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="64"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="66"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
@@ -3499,15 +3466,15 @@
     </row>
     <row r="11" spans="1:21" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="64"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="66"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
@@ -3518,18 +3485,18 @@
       <c r="R11" s="13"/>
     </row>
     <row r="12" spans="1:21" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="67" t="s">
         <v>112</v>
       </c>
-      <c r="B12" s="66"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68"/>
       <c r="K12" s="37"/>
       <c r="L12" s="37"/>
       <c r="M12" s="37"/>
@@ -3724,16 +3691,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="B7:J7"/>
     <mergeCell ref="B8:J8"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
     <mergeCell ref="A12:J12"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="B7:J7"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
@@ -3768,34 +3735,36 @@
   </sheetPr>
   <dimension ref="A1:W60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="14" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="75" workbookViewId="0">
+      <pane xSplit="1" ySplit="14" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="J38" sqref="J38"/>
+      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.875" customWidth="1"/>
-    <col min="2" max="10" width="24.625" customWidth="1"/>
-    <col min="11" max="11" width="23.25" customWidth="1"/>
+    <col min="2" max="2" width="24.625" hidden="1" customWidth="1"/>
+    <col min="3" max="5" width="24.625" customWidth="1"/>
+    <col min="6" max="10" width="24.625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="23.25" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="3.375" hidden="1" customWidth="1"/>
     <col min="13" max="18" width="24.625" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="35.5" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="64.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>111</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="F1" s="90" t="s">
+      <c r="F1" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="G1" s="60" t="s">
         <v>195</v>
       </c>
       <c r="H1" s="33"/>
@@ -3814,267 +3783,267 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="23.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="83" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="80"/>
-      <c r="O3" s="80"/>
-      <c r="P3" s="80"/>
-      <c r="Q3" s="80"/>
-      <c r="R3" s="80"/>
-      <c r="S3" s="80"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="84"/>
     </row>
     <row r="4" spans="1:23" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="87" t="s">
         <v>115</v>
       </c>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="84"/>
-      <c r="M4" s="84"/>
-      <c r="N4" s="84"/>
-      <c r="O4" s="84"/>
-      <c r="P4" s="84"/>
-      <c r="Q4" s="84"/>
-      <c r="R4" s="84"/>
-      <c r="S4" s="84"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="88"/>
+      <c r="P4" s="88"/>
+      <c r="Q4" s="88"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
     </row>
     <row r="5" spans="1:23" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="87" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
-      <c r="L5" s="84"/>
-      <c r="M5" s="84"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="84"/>
-      <c r="P5" s="84"/>
-      <c r="Q5" s="84"/>
-      <c r="R5" s="84"/>
-      <c r="S5" s="84"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="88"/>
+      <c r="M5" s="88"/>
+      <c r="N5" s="88"/>
+      <c r="O5" s="88"/>
+      <c r="P5" s="88"/>
+      <c r="Q5" s="88"/>
+      <c r="R5" s="88"/>
+      <c r="S5" s="88"/>
     </row>
     <row r="6" spans="1:23" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="83" t="s">
+      <c r="B6" s="87" t="s">
         <v>118</v>
       </c>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="84"/>
-      <c r="N6" s="84"/>
-      <c r="O6" s="84"/>
-      <c r="P6" s="84"/>
-      <c r="Q6" s="84"/>
-      <c r="R6" s="84"/>
-      <c r="S6" s="84"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="88"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="88"/>
+      <c r="M6" s="88"/>
+      <c r="N6" s="88"/>
+      <c r="O6" s="88"/>
+      <c r="P6" s="88"/>
+      <c r="Q6" s="88"/>
+      <c r="R6" s="88"/>
+      <c r="S6" s="88"/>
     </row>
     <row r="7" spans="1:23" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B7" s="83" t="s">
+      <c r="B7" s="87" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="84"/>
-      <c r="J7" s="84"/>
-      <c r="K7" s="84"/>
-      <c r="L7" s="84"/>
-      <c r="M7" s="84"/>
-      <c r="N7" s="84"/>
-      <c r="O7" s="84"/>
-      <c r="P7" s="84"/>
-      <c r="Q7" s="84"/>
-      <c r="R7" s="84"/>
-      <c r="S7" s="84"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="88"/>
+      <c r="J7" s="88"/>
+      <c r="K7" s="88"/>
+      <c r="L7" s="88"/>
+      <c r="M7" s="88"/>
+      <c r="N7" s="88"/>
+      <c r="O7" s="88"/>
+      <c r="P7" s="88"/>
+      <c r="Q7" s="88"/>
+      <c r="R7" s="88"/>
+      <c r="S7" s="88"/>
     </row>
     <row r="8" spans="1:23" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B8" s="83" t="s">
+      <c r="B8" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="84"/>
-      <c r="J8" s="84"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="84"/>
-      <c r="M8" s="84"/>
-      <c r="N8" s="84"/>
-      <c r="O8" s="84"/>
-      <c r="P8" s="84"/>
-      <c r="Q8" s="84"/>
-      <c r="R8" s="84"/>
-      <c r="S8" s="84"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="88"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="88"/>
+      <c r="N8" s="88"/>
+      <c r="O8" s="88"/>
+      <c r="P8" s="88"/>
+      <c r="Q8" s="88"/>
+      <c r="R8" s="88"/>
+      <c r="S8" s="88"/>
     </row>
     <row r="9" spans="1:23" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="54" t="s">
         <v>173</v>
       </c>
-      <c r="B9" s="83" t="s">
+      <c r="B9" s="87" t="s">
         <v>174</v>
       </c>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="84"/>
-      <c r="K9" s="84"/>
-      <c r="L9" s="84"/>
-      <c r="M9" s="84"/>
-      <c r="N9" s="84"/>
-      <c r="O9" s="84"/>
-      <c r="P9" s="84"/>
-      <c r="Q9" s="84"/>
-      <c r="R9" s="84"/>
-      <c r="S9" s="84"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="88"/>
+      <c r="K9" s="88"/>
+      <c r="L9" s="88"/>
+      <c r="M9" s="88"/>
+      <c r="N9" s="88"/>
+      <c r="O9" s="88"/>
+      <c r="P9" s="88"/>
+      <c r="Q9" s="88"/>
+      <c r="R9" s="88"/>
+      <c r="S9" s="88"/>
     </row>
     <row r="10" spans="1:23" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="87" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
-      <c r="J10" s="84"/>
-      <c r="K10" s="84"/>
-      <c r="L10" s="84"/>
-      <c r="M10" s="84"/>
-      <c r="N10" s="84"/>
-      <c r="O10" s="84"/>
-      <c r="P10" s="84"/>
-      <c r="Q10" s="84"/>
-      <c r="R10" s="84"/>
-      <c r="S10" s="84"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="88"/>
+      <c r="L10" s="88"/>
+      <c r="M10" s="88"/>
+      <c r="N10" s="88"/>
+      <c r="O10" s="88"/>
+      <c r="P10" s="88"/>
+      <c r="Q10" s="88"/>
+      <c r="R10" s="88"/>
+      <c r="S10" s="88"/>
     </row>
     <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="85"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="86"/>
-      <c r="L11" s="86"/>
-      <c r="M11" s="86"/>
-      <c r="N11" s="86"/>
-      <c r="O11" s="86"/>
-      <c r="P11" s="86"/>
-      <c r="Q11" s="86"/>
-      <c r="R11" s="86"/>
-      <c r="S11" s="86"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="90"/>
+      <c r="I11" s="90"/>
+      <c r="J11" s="90"/>
+      <c r="K11" s="90"/>
+      <c r="L11" s="90"/>
+      <c r="M11" s="90"/>
+      <c r="N11" s="90"/>
+      <c r="O11" s="90"/>
+      <c r="P11" s="90"/>
+      <c r="Q11" s="90"/>
+      <c r="R11" s="90"/>
+      <c r="S11" s="90"/>
     </row>
     <row r="12" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="85"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="86"/>
-      <c r="L12" s="86"/>
-      <c r="M12" s="86"/>
-      <c r="N12" s="86"/>
-      <c r="O12" s="86"/>
-      <c r="P12" s="86"/>
-      <c r="Q12" s="86"/>
-      <c r="R12" s="86"/>
-      <c r="S12" s="86"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="90"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="90"/>
+      <c r="L12" s="90"/>
+      <c r="M12" s="90"/>
+      <c r="N12" s="90"/>
+      <c r="O12" s="90"/>
+      <c r="P12" s="90"/>
+      <c r="Q12" s="90"/>
+      <c r="R12" s="90"/>
+      <c r="S12" s="90"/>
     </row>
     <row r="13" spans="1:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="85" t="s">
         <v>112</v>
       </c>
-      <c r="B13" s="82"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="82"/>
-      <c r="I13" s="82"/>
-      <c r="J13" s="82"/>
-      <c r="K13" s="82"/>
-      <c r="L13" s="82"/>
-      <c r="M13" s="82"/>
-      <c r="N13" s="82"/>
-      <c r="O13" s="82"/>
-      <c r="P13" s="82"/>
-      <c r="Q13" s="82"/>
-      <c r="R13" s="82"/>
-      <c r="S13" s="82"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="86"/>
+      <c r="J13" s="86"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="86"/>
+      <c r="M13" s="86"/>
+      <c r="N13" s="86"/>
+      <c r="O13" s="86"/>
+      <c r="P13" s="86"/>
+      <c r="Q13" s="86"/>
+      <c r="R13" s="86"/>
+      <c r="S13" s="86"/>
     </row>
     <row r="14" spans="1:23" s="3" customFormat="1" ht="70.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -4184,16 +4153,16 @@
       <c r="A16" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="91" t="s">
+      <c r="B16" s="62" t="s">
         <v>208</v>
       </c>
       <c r="C16" s="59" t="s">
         <v>203</v>
       </c>
-      <c r="D16" s="91" t="s">
+      <c r="D16" s="62" t="s">
         <v>202</v>
       </c>
-      <c r="E16" s="91" t="s">
+      <c r="E16" s="62" t="s">
         <v>204</v>
       </c>
       <c r="F16" s="51" t="s">
@@ -4208,7 +4177,7 @@
       <c r="I16" s="52" t="s">
         <v>201</v>
       </c>
-      <c r="J16" s="92" t="s">
+      <c r="J16" s="63" t="s">
         <v>207</v>
       </c>
       <c r="K16" s="16"/>
@@ -5274,86 +5243,86 @@
     </row>
     <row r="44" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45" s="67" t="s">
+      <c r="A45" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="B45" s="68"/>
-      <c r="C45" s="68"/>
-      <c r="D45" s="68"/>
-      <c r="E45" s="68"/>
-      <c r="F45" s="68"/>
-      <c r="G45" s="68"/>
-      <c r="H45" s="68"/>
-      <c r="I45" s="68"/>
-      <c r="J45" s="68"/>
-      <c r="K45" s="68"/>
-      <c r="L45" s="68"/>
-      <c r="M45" s="68"/>
-      <c r="N45" s="68"/>
-      <c r="O45" s="68"/>
-      <c r="P45" s="68"/>
-      <c r="Q45" s="68"/>
-      <c r="R45" s="69"/>
+      <c r="B45" s="72"/>
+      <c r="C45" s="72"/>
+      <c r="D45" s="72"/>
+      <c r="E45" s="72"/>
+      <c r="F45" s="72"/>
+      <c r="G45" s="72"/>
+      <c r="H45" s="72"/>
+      <c r="I45" s="72"/>
+      <c r="J45" s="72"/>
+      <c r="K45" s="72"/>
+      <c r="L45" s="72"/>
+      <c r="M45" s="72"/>
+      <c r="N45" s="72"/>
+      <c r="O45" s="72"/>
+      <c r="P45" s="72"/>
+      <c r="Q45" s="72"/>
+      <c r="R45" s="73"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A46" s="70"/>
-      <c r="B46" s="71"/>
-      <c r="C46" s="71"/>
-      <c r="D46" s="71"/>
-      <c r="E46" s="71"/>
-      <c r="F46" s="71"/>
-      <c r="G46" s="71"/>
-      <c r="H46" s="71"/>
-      <c r="I46" s="71"/>
-      <c r="J46" s="71"/>
-      <c r="K46" s="71"/>
-      <c r="L46" s="71"/>
-      <c r="M46" s="71"/>
-      <c r="N46" s="71"/>
-      <c r="O46" s="71"/>
-      <c r="P46" s="71"/>
-      <c r="Q46" s="71"/>
-      <c r="R46" s="72"/>
+      <c r="A46" s="74"/>
+      <c r="B46" s="75"/>
+      <c r="C46" s="75"/>
+      <c r="D46" s="75"/>
+      <c r="E46" s="75"/>
+      <c r="F46" s="75"/>
+      <c r="G46" s="75"/>
+      <c r="H46" s="75"/>
+      <c r="I46" s="75"/>
+      <c r="J46" s="75"/>
+      <c r="K46" s="75"/>
+      <c r="L46" s="75"/>
+      <c r="M46" s="75"/>
+      <c r="N46" s="75"/>
+      <c r="O46" s="75"/>
+      <c r="P46" s="75"/>
+      <c r="Q46" s="75"/>
+      <c r="R46" s="76"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47" s="70"/>
-      <c r="B47" s="71"/>
-      <c r="C47" s="71"/>
-      <c r="D47" s="71"/>
-      <c r="E47" s="71"/>
-      <c r="F47" s="71"/>
-      <c r="G47" s="71"/>
-      <c r="H47" s="71"/>
-      <c r="I47" s="71"/>
-      <c r="J47" s="71"/>
-      <c r="K47" s="71"/>
-      <c r="L47" s="71"/>
-      <c r="M47" s="71"/>
-      <c r="N47" s="71"/>
-      <c r="O47" s="71"/>
-      <c r="P47" s="71"/>
-      <c r="Q47" s="71"/>
-      <c r="R47" s="72"/>
+      <c r="A47" s="74"/>
+      <c r="B47" s="75"/>
+      <c r="C47" s="75"/>
+      <c r="D47" s="75"/>
+      <c r="E47" s="75"/>
+      <c r="F47" s="75"/>
+      <c r="G47" s="75"/>
+      <c r="H47" s="75"/>
+      <c r="I47" s="75"/>
+      <c r="J47" s="75"/>
+      <c r="K47" s="75"/>
+      <c r="L47" s="75"/>
+      <c r="M47" s="75"/>
+      <c r="N47" s="75"/>
+      <c r="O47" s="75"/>
+      <c r="P47" s="75"/>
+      <c r="Q47" s="75"/>
+      <c r="R47" s="76"/>
     </row>
     <row r="48" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="73"/>
-      <c r="B48" s="74"/>
-      <c r="C48" s="74"/>
-      <c r="D48" s="74"/>
-      <c r="E48" s="74"/>
-      <c r="F48" s="74"/>
-      <c r="G48" s="74"/>
-      <c r="H48" s="74"/>
-      <c r="I48" s="74"/>
-      <c r="J48" s="74"/>
-      <c r="K48" s="74"/>
-      <c r="L48" s="74"/>
-      <c r="M48" s="74"/>
-      <c r="N48" s="74"/>
-      <c r="O48" s="74"/>
-      <c r="P48" s="74"/>
-      <c r="Q48" s="74"/>
-      <c r="R48" s="75"/>
+      <c r="A48" s="77"/>
+      <c r="B48" s="78"/>
+      <c r="C48" s="78"/>
+      <c r="D48" s="78"/>
+      <c r="E48" s="78"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="78"/>
+      <c r="H48" s="78"/>
+      <c r="I48" s="78"/>
+      <c r="J48" s="78"/>
+      <c r="K48" s="78"/>
+      <c r="L48" s="78"/>
+      <c r="M48" s="78"/>
+      <c r="N48" s="78"/>
+      <c r="O48" s="78"/>
+      <c r="P48" s="78"/>
+      <c r="Q48" s="78"/>
+      <c r="R48" s="79"/>
     </row>
     <row r="49" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -5376,26 +5345,26 @@
       </c>
     </row>
     <row r="54" spans="1:18" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="76" t="s">
+      <c r="A54" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="77"/>
-      <c r="C54" s="77"/>
-      <c r="D54" s="77"/>
-      <c r="E54" s="77"/>
-      <c r="F54" s="77"/>
-      <c r="G54" s="77"/>
-      <c r="H54" s="77"/>
-      <c r="I54" s="77"/>
-      <c r="J54" s="77"/>
-      <c r="K54" s="77"/>
-      <c r="L54" s="77"/>
-      <c r="M54" s="77"/>
-      <c r="N54" s="77"/>
-      <c r="O54" s="77"/>
-      <c r="P54" s="77"/>
-      <c r="Q54" s="77"/>
-      <c r="R54" s="78"/>
+      <c r="B54" s="81"/>
+      <c r="C54" s="81"/>
+      <c r="D54" s="81"/>
+      <c r="E54" s="81"/>
+      <c r="F54" s="81"/>
+      <c r="G54" s="81"/>
+      <c r="H54" s="81"/>
+      <c r="I54" s="81"/>
+      <c r="J54" s="81"/>
+      <c r="K54" s="81"/>
+      <c r="L54" s="81"/>
+      <c r="M54" s="81"/>
+      <c r="N54" s="81"/>
+      <c r="O54" s="81"/>
+      <c r="P54" s="81"/>
+      <c r="Q54" s="81"/>
+      <c r="R54" s="82"/>
     </row>
     <row r="55" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="57" t="s">
@@ -5463,90 +5432,90 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="Q27 B27:J28">
-    <cfRule type="containsText" dxfId="59" priority="54" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="56" priority="54" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",B27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="55" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="55" priority="55" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",B27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="56" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="54" priority="56" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",B27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P27">
-    <cfRule type="containsText" dxfId="56" priority="51" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="53" priority="51" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",P27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="52" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="52" priority="52" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",P27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="53" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="51" priority="53" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",P27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:J26">
-    <cfRule type="containsText" dxfId="53" priority="1" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="50" priority="1" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",B17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="49" priority="2" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",B17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="48" priority="3" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17:P22">
-    <cfRule type="containsText" dxfId="50" priority="16" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="47" priority="16" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",P17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="17" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="46" priority="17" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",P17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="18" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="45" priority="18" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",P17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O23:Q23 Q17:Q22">
-    <cfRule type="containsText" dxfId="47" priority="13" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="44" priority="13" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",O17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="14" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="43" priority="14" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",O17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="15" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="42" priority="15" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",O17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q25">
-    <cfRule type="containsText" dxfId="44" priority="10" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="41" priority="10" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",Q25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="11" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="40" priority="11" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",Q25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="12" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="39" priority="12" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",Q25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L23">
-    <cfRule type="containsText" dxfId="41" priority="7" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="38" priority="7" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",L23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="8" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="37" priority="8" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",L23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="9" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="36" priority="9" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",L23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:K23">
-    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="35" priority="4" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",K17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="34" priority="5" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",K17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="33" priority="6" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",K17)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5627,236 +5596,236 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="83" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="80"/>
-      <c r="O3" s="80"/>
-      <c r="P3" s="80"/>
-      <c r="Q3" s="80"/>
-      <c r="R3" s="80"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="84"/>
     </row>
     <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="91" t="s">
         <v>115</v>
       </c>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87"/>
-      <c r="I4" s="87"/>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
-      <c r="M4" s="87"/>
-      <c r="N4" s="87"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="87"/>
-      <c r="Q4" s="87"/>
-      <c r="R4" s="87"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="91"/>
+      <c r="Q4" s="91"/>
+      <c r="R4" s="91"/>
     </row>
     <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="91" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
-      <c r="L5" s="87"/>
-      <c r="M5" s="87"/>
-      <c r="N5" s="87"/>
-      <c r="O5" s="87"/>
-      <c r="P5" s="87"/>
-      <c r="Q5" s="87"/>
-      <c r="R5" s="87"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="91"/>
+      <c r="L5" s="91"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="91"/>
+      <c r="O5" s="91"/>
+      <c r="P5" s="91"/>
+      <c r="Q5" s="91"/>
+      <c r="R5" s="91"/>
     </row>
     <row r="6" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="91" t="s">
         <v>118</v>
       </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="87"/>
-      <c r="K6" s="87"/>
-      <c r="L6" s="87"/>
-      <c r="M6" s="87"/>
-      <c r="N6" s="87"/>
-      <c r="O6" s="87"/>
-      <c r="P6" s="87"/>
-      <c r="Q6" s="87"/>
-      <c r="R6" s="87"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+      <c r="O6" s="91"/>
+      <c r="P6" s="91"/>
+      <c r="Q6" s="91"/>
+      <c r="R6" s="91"/>
     </row>
     <row r="7" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B7" s="87" t="s">
+      <c r="B7" s="91" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="87"/>
-      <c r="L7" s="87"/>
-      <c r="M7" s="87"/>
-      <c r="N7" s="87"/>
-      <c r="O7" s="87"/>
-      <c r="P7" s="87"/>
-      <c r="Q7" s="87"/>
-      <c r="R7" s="87"/>
+      <c r="C7" s="91"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="91"/>
+      <c r="H7" s="91"/>
+      <c r="I7" s="91"/>
+      <c r="J7" s="91"/>
+      <c r="K7" s="91"/>
+      <c r="L7" s="91"/>
+      <c r="M7" s="91"/>
+      <c r="N7" s="91"/>
+      <c r="O7" s="91"/>
+      <c r="P7" s="91"/>
+      <c r="Q7" s="91"/>
+      <c r="R7" s="91"/>
     </row>
     <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B8" s="87" t="s">
+      <c r="B8" s="91" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="87"/>
-      <c r="D8" s="87"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="87"/>
-      <c r="G8" s="87"/>
-      <c r="H8" s="87"/>
-      <c r="I8" s="87"/>
-      <c r="J8" s="87"/>
-      <c r="K8" s="87"/>
-      <c r="L8" s="87"/>
-      <c r="M8" s="87"/>
-      <c r="N8" s="87"/>
-      <c r="O8" s="87"/>
-      <c r="P8" s="87"/>
-      <c r="Q8" s="87"/>
-      <c r="R8" s="87"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="91"/>
+      <c r="G8" s="91"/>
+      <c r="H8" s="91"/>
+      <c r="I8" s="91"/>
+      <c r="J8" s="91"/>
+      <c r="K8" s="91"/>
+      <c r="L8" s="91"/>
+      <c r="M8" s="91"/>
+      <c r="N8" s="91"/>
+      <c r="O8" s="91"/>
+      <c r="P8" s="91"/>
+      <c r="Q8" s="91"/>
+      <c r="R8" s="91"/>
     </row>
     <row r="9" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="54" t="s">
         <v>173</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="64" t="s">
         <v>174</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="63"/>
-      <c r="M9" s="63"/>
-      <c r="N9" s="63"/>
-      <c r="O9" s="63"/>
-      <c r="P9" s="63"/>
-      <c r="Q9" s="63"/>
-      <c r="R9" s="63"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="65"/>
+      <c r="L9" s="65"/>
+      <c r="M9" s="65"/>
+      <c r="N9" s="65"/>
+      <c r="O9" s="65"/>
+      <c r="P9" s="65"/>
+      <c r="Q9" s="65"/>
+      <c r="R9" s="65"/>
     </row>
     <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B10" s="87" t="s">
+      <c r="B10" s="91" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="87"/>
-      <c r="D10" s="87"/>
-      <c r="E10" s="87"/>
-      <c r="F10" s="87"/>
-      <c r="G10" s="87"/>
-      <c r="H10" s="87"/>
-      <c r="I10" s="87"/>
-      <c r="J10" s="87"/>
-      <c r="K10" s="87"/>
-      <c r="L10" s="87"/>
-      <c r="M10" s="87"/>
-      <c r="N10" s="87"/>
-      <c r="O10" s="87"/>
-      <c r="P10" s="87"/>
-      <c r="Q10" s="87"/>
-      <c r="R10" s="87"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
+      <c r="H10" s="91"/>
+      <c r="I10" s="91"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91"/>
+      <c r="L10" s="91"/>
+      <c r="M10" s="91"/>
+      <c r="N10" s="91"/>
+      <c r="O10" s="91"/>
+      <c r="P10" s="91"/>
+      <c r="Q10" s="91"/>
+      <c r="R10" s="91"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="88"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="88"/>
-      <c r="K11" s="88"/>
-      <c r="L11" s="88"/>
-      <c r="M11" s="88"/>
-      <c r="N11" s="88"/>
-      <c r="O11" s="88"/>
-      <c r="P11" s="88"/>
-      <c r="Q11" s="88"/>
-      <c r="R11" s="88"/>
+      <c r="B11" s="92"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="92"/>
+      <c r="F11" s="92"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="92"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="92"/>
+      <c r="K11" s="92"/>
+      <c r="L11" s="92"/>
+      <c r="M11" s="92"/>
+      <c r="N11" s="92"/>
+      <c r="O11" s="92"/>
+      <c r="P11" s="92"/>
+      <c r="Q11" s="92"/>
+      <c r="R11" s="92"/>
     </row>
     <row r="12" spans="1:18" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="85" t="s">
         <v>112</v>
       </c>
-      <c r="B12" s="82"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="82"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="82"/>
-      <c r="H12" s="82"/>
-      <c r="I12" s="82"/>
-      <c r="J12" s="82"/>
-      <c r="K12" s="82"/>
-      <c r="L12" s="82"/>
-      <c r="M12" s="82"/>
-      <c r="N12" s="82"/>
-      <c r="O12" s="82"/>
-      <c r="P12" s="82"/>
-      <c r="Q12" s="82"/>
-      <c r="R12" s="82"/>
+      <c r="B12" s="86"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="86"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="86"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="86"/>
+      <c r="R12" s="86"/>
     </row>
     <row r="13" spans="1:18" s="3" customFormat="1" ht="70.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="55" t="s">
@@ -6879,88 +6848,88 @@
     </row>
     <row r="41" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="67" t="s">
+      <c r="A42" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="B42" s="68"/>
-      <c r="C42" s="68"/>
-      <c r="D42" s="68"/>
-      <c r="E42" s="68"/>
-      <c r="F42" s="68"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="68"/>
-      <c r="I42" s="68"/>
-      <c r="J42" s="68"/>
-      <c r="K42" s="68"/>
-      <c r="L42" s="68"/>
-      <c r="M42" s="68"/>
-      <c r="N42" s="68"/>
-      <c r="O42" s="68"/>
-      <c r="P42" s="68"/>
-      <c r="Q42" s="69"/>
+      <c r="B42" s="72"/>
+      <c r="C42" s="72"/>
+      <c r="D42" s="72"/>
+      <c r="E42" s="72"/>
+      <c r="F42" s="72"/>
+      <c r="G42" s="72"/>
+      <c r="H42" s="72"/>
+      <c r="I42" s="72"/>
+      <c r="J42" s="72"/>
+      <c r="K42" s="72"/>
+      <c r="L42" s="72"/>
+      <c r="M42" s="72"/>
+      <c r="N42" s="72"/>
+      <c r="O42" s="72"/>
+      <c r="P42" s="72"/>
+      <c r="Q42" s="73"/>
       <c r="S42"/>
       <c r="T42"/>
     </row>
     <row r="43" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="70"/>
-      <c r="B43" s="71"/>
-      <c r="C43" s="71"/>
-      <c r="D43" s="71"/>
-      <c r="E43" s="71"/>
-      <c r="F43" s="71"/>
-      <c r="G43" s="71"/>
-      <c r="H43" s="71"/>
-      <c r="I43" s="71"/>
-      <c r="J43" s="71"/>
-      <c r="K43" s="71"/>
-      <c r="L43" s="71"/>
-      <c r="M43" s="71"/>
-      <c r="N43" s="71"/>
-      <c r="O43" s="71"/>
-      <c r="P43" s="71"/>
-      <c r="Q43" s="72"/>
+      <c r="A43" s="74"/>
+      <c r="B43" s="75"/>
+      <c r="C43" s="75"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="75"/>
+      <c r="F43" s="75"/>
+      <c r="G43" s="75"/>
+      <c r="H43" s="75"/>
+      <c r="I43" s="75"/>
+      <c r="J43" s="75"/>
+      <c r="K43" s="75"/>
+      <c r="L43" s="75"/>
+      <c r="M43" s="75"/>
+      <c r="N43" s="75"/>
+      <c r="O43" s="75"/>
+      <c r="P43" s="75"/>
+      <c r="Q43" s="76"/>
       <c r="S43"/>
       <c r="T43"/>
     </row>
     <row r="44" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="70"/>
-      <c r="B44" s="71"/>
-      <c r="C44" s="71"/>
-      <c r="D44" s="71"/>
-      <c r="E44" s="71"/>
-      <c r="F44" s="71"/>
-      <c r="G44" s="71"/>
-      <c r="H44" s="71"/>
-      <c r="I44" s="71"/>
-      <c r="J44" s="71"/>
-      <c r="K44" s="71"/>
-      <c r="L44" s="71"/>
-      <c r="M44" s="71"/>
-      <c r="N44" s="71"/>
-      <c r="O44" s="71"/>
-      <c r="P44" s="71"/>
-      <c r="Q44" s="72"/>
+      <c r="A44" s="74"/>
+      <c r="B44" s="75"/>
+      <c r="C44" s="75"/>
+      <c r="D44" s="75"/>
+      <c r="E44" s="75"/>
+      <c r="F44" s="75"/>
+      <c r="G44" s="75"/>
+      <c r="H44" s="75"/>
+      <c r="I44" s="75"/>
+      <c r="J44" s="75"/>
+      <c r="K44" s="75"/>
+      <c r="L44" s="75"/>
+      <c r="M44" s="75"/>
+      <c r="N44" s="75"/>
+      <c r="O44" s="75"/>
+      <c r="P44" s="75"/>
+      <c r="Q44" s="76"/>
       <c r="S44"/>
       <c r="T44"/>
     </row>
     <row r="45" spans="1:20" s="17" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="73"/>
-      <c r="B45" s="74"/>
-      <c r="C45" s="74"/>
-      <c r="D45" s="74"/>
-      <c r="E45" s="74"/>
-      <c r="F45" s="74"/>
-      <c r="G45" s="74"/>
-      <c r="H45" s="74"/>
-      <c r="I45" s="74"/>
-      <c r="J45" s="74"/>
-      <c r="K45" s="74"/>
-      <c r="L45" s="74"/>
-      <c r="M45" s="74"/>
-      <c r="N45" s="74"/>
-      <c r="O45" s="74"/>
-      <c r="P45" s="74"/>
-      <c r="Q45" s="75"/>
+      <c r="A45" s="77"/>
+      <c r="B45" s="78"/>
+      <c r="C45" s="78"/>
+      <c r="D45" s="78"/>
+      <c r="E45" s="78"/>
+      <c r="F45" s="78"/>
+      <c r="G45" s="78"/>
+      <c r="H45" s="78"/>
+      <c r="I45" s="78"/>
+      <c r="J45" s="78"/>
+      <c r="K45" s="78"/>
+      <c r="L45" s="78"/>
+      <c r="M45" s="78"/>
+      <c r="N45" s="78"/>
+      <c r="O45" s="78"/>
+      <c r="P45" s="78"/>
+      <c r="Q45" s="79"/>
       <c r="S45"/>
       <c r="T45"/>
     </row>
@@ -7078,35 +7047,30 @@
       <c r="T50"/>
     </row>
     <row r="51" spans="1:20" s="17" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="76" t="s">
+      <c r="A51" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="77"/>
-      <c r="C51" s="77"/>
-      <c r="D51" s="77"/>
-      <c r="E51" s="77"/>
-      <c r="F51" s="77"/>
-      <c r="G51" s="77"/>
-      <c r="H51" s="77"/>
-      <c r="I51" s="77"/>
-      <c r="J51" s="77"/>
-      <c r="K51" s="77"/>
-      <c r="L51" s="77"/>
-      <c r="M51" s="77"/>
-      <c r="N51" s="77"/>
-      <c r="O51" s="77"/>
-      <c r="P51" s="77"/>
-      <c r="Q51" s="78"/>
+      <c r="B51" s="81"/>
+      <c r="C51" s="81"/>
+      <c r="D51" s="81"/>
+      <c r="E51" s="81"/>
+      <c r="F51" s="81"/>
+      <c r="G51" s="81"/>
+      <c r="H51" s="81"/>
+      <c r="I51" s="81"/>
+      <c r="J51" s="81"/>
+      <c r="K51" s="81"/>
+      <c r="L51" s="81"/>
+      <c r="M51" s="81"/>
+      <c r="N51" s="81"/>
+      <c r="O51" s="81"/>
+      <c r="P51" s="81"/>
+      <c r="Q51" s="82"/>
       <c r="S51"/>
       <c r="T51"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A51:Q51"/>
-    <mergeCell ref="B10:R10"/>
-    <mergeCell ref="B11:R11"/>
-    <mergeCell ref="A12:R12"/>
-    <mergeCell ref="A42:Q45"/>
     <mergeCell ref="B9:R9"/>
     <mergeCell ref="B8:R8"/>
     <mergeCell ref="A3:R3"/>
@@ -7114,126 +7078,131 @@
     <mergeCell ref="B5:R5"/>
     <mergeCell ref="B6:R6"/>
     <mergeCell ref="B7:R7"/>
+    <mergeCell ref="A51:Q51"/>
+    <mergeCell ref="B10:R10"/>
+    <mergeCell ref="B11:R11"/>
+    <mergeCell ref="A12:R12"/>
+    <mergeCell ref="A42:Q45"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="O16:O21">
-    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",O16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",O16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",O16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22:P22 P16:P21">
-    <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",N16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",N16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="27" priority="33" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",N16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P26">
-    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",P26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",P26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",P26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O26">
-    <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",O26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",O26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",O26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P24">
-    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",P24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",P24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",P24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22">
-    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",K22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",K22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",K22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:J22">
-    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",J16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",J16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",J16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:F26">
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",B26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",B26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",B26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:F27">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",B27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",B27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",B27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:I27">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",G26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",G26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",G26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16:I25">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",G16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",G16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",G16)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>